<commit_message>
corrected original_id in metadata
</commit_message>
<xml_diff>
--- a/data/metadata/metadata.xlsx
+++ b/data/metadata/metadata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Spatial transcriptomic experiments\Davide_Analyses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marusa/Documents/spatial_prions/data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE88A46-DB51-5A4A-9DA6-D960EEEBB2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,21 +87,12 @@
     <t>o2885711-NBH_hyp_control</t>
   </si>
   <si>
-    <t>o2885711-ME7_hyp</t>
-  </si>
-  <si>
     <t>ME7</t>
   </si>
   <si>
-    <t>o2885711-mNS_hyp</t>
-  </si>
-  <si>
     <t>mNS</t>
   </si>
   <si>
-    <t>o2885711-RML6_hyp</t>
-  </si>
-  <si>
     <t>V11M16-057</t>
   </si>
   <si>
@@ -162,12 +154,21 @@
   </si>
   <si>
     <t>RML6_30_2</t>
+  </si>
+  <si>
+    <t>o2885712-ME7_hyp</t>
+  </si>
+  <si>
+    <t>o2885713-mNS_hyp</t>
+  </si>
+  <si>
+    <t>o2885714-RML6_hyp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -480,28 +481,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -522,12 +523,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1">
         <v>27</v>
@@ -542,18 +543,18 @@
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1">
         <v>27</v>
@@ -568,18 +569,18 @@
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -594,18 +595,18 @@
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -620,18 +621,18 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1">
         <v>30</v>
@@ -646,18 +647,18 @@
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1">
         <v>30</v>
@@ -672,18 +673,18 @@
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -698,18 +699,18 @@
         <v>3</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
         <v>28</v>
       </c>
-      <c r="H8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -724,18 +725,18 @@
         <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1">
         <v>30</v>
@@ -750,24 +751,24 @@
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1">
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>9</v>
@@ -776,24 +777,24 @@
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1">
         <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>9</v>
@@ -802,18 +803,18 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1">
         <v>30</v>
@@ -828,10 +829,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
         <v>29</v>
-      </c>
-      <c r="H13" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>